<commit_message>
fixed triangle positions as per #880
</commit_message>
<xml_diff>
--- a/app/skinGui/iniGenerators/rightLeg_Lower_ini_generator.xlsx
+++ b/app/skinGui/iniGenerators/rightLeg_Lower_ini_generator.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\robotologia\icub-main\app\skinGui\iniGenerators\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12585" yWindow="-15" windowWidth="12630" windowHeight="12000" activeTab="5"/>
+    <workbookView xWindow="12585" yWindow="-15" windowWidth="12630" windowHeight="12000" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="4535A" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
     <sheet name="4616A" sheetId="8" r:id="rId7"/>
     <sheet name="final ini" sheetId="5" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -131,7 +136,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -851,6 +856,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -16685,7 +16693,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -16720,7 +16728,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -16932,7 +16940,7 @@
   <dimension ref="A1:U55"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17579,26 +17587,26 @@
         <v>26</v>
       </c>
       <c r="B17" s="61">
-        <f>((ROUND($L17/10,0))-1)*4+MOD($L17,10)+((J17-1)*16)</f>
+        <f t="shared" ref="B17:B24" si="2">((ROUND($L17/10,0))-1)*4+MOD($L17,10)+((J17-1)*16)</f>
         <v>3</v>
       </c>
       <c r="C17" s="61">
-        <f t="shared" ref="C17:C24" si="2">((+P17*COS($O$3)-Q17*SIN($O$3)+$O$7)*$S$3)</f>
+        <f t="shared" ref="C17:C24" si="3">((+P17*COS($O$3)-Q17*SIN($O$3)+$O$7)*$S$3)</f>
         <v>63.602540378443734</v>
       </c>
       <c r="D17" s="61">
-        <f t="shared" ref="D17:D24" si="3">((P17*SIN($O$3)+Q17*COS($O$3)+$O$9)*$S$4)</f>
+        <f t="shared" ref="D17:D24" si="4">((P17*SIN($O$3)+Q17*COS($O$3)+$O$9)*$S$4)</f>
         <v>9.5854811567261606</v>
       </c>
       <c r="E17" s="61">
-        <f t="shared" ref="E17:E24" si="4">IF(($S$3*$S$4)=1,1,-1)*(($N17/3.1416*180)+$O$5)</f>
+        <f t="shared" ref="E17:E24" si="5">IF(($S$3*$S$4)=1,1,-1)*(($N17/3.1416*180)+$O$5)</f>
         <v>-1.403057715734235E-4</v>
       </c>
       <c r="F17" s="60">
         <v>5</v>
       </c>
       <c r="G17" s="63">
-        <f>IF($S$3*$S$4=-1,1,0)</f>
+        <f t="shared" ref="G17:G24" si="6">IF($S$3*$S$4=-1,1,0)</f>
         <v>0</v>
       </c>
       <c r="I17" s="1"/>
@@ -17631,26 +17639,26 @@
         <v>26</v>
       </c>
       <c r="B18" s="61">
-        <f>((ROUND($L18/10,0))-1)*4+MOD($L18,10)+((J18-1)*16)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="C18" s="61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>47.602540378443763</v>
       </c>
       <c r="D18" s="61">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>18.823085463760165</v>
       </c>
       <c r="E18" s="61">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>59.999719388456853</v>
       </c>
       <c r="F18" s="60">
         <v>5</v>
       </c>
       <c r="G18" s="63">
-        <f>IF($S$3*$S$4=-1,1,0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I18" s="1"/>
@@ -17683,26 +17691,26 @@
         <v>26</v>
       </c>
       <c r="B19" s="61">
-        <f>((ROUND($L19/10,0))-1)*4+MOD($L19,10)+((J19-1)*16)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="C19" s="61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>31.602540378443791</v>
       </c>
       <c r="D19" s="61">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-8.8897274573418485</v>
       </c>
       <c r="E19" s="61">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>59.999719388456853</v>
       </c>
       <c r="F19" s="60">
         <v>5</v>
       </c>
       <c r="G19" s="63">
-        <f>IF($S$3*$S$4=-1,1,0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I19" s="1"/>
@@ -17735,26 +17743,26 @@
         <v>26</v>
       </c>
       <c r="B20" s="61">
-        <f>((ROUND($L20/10,0))-1)*4+MOD($L20,10)+((J20-1)*16)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="C20" s="61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>31.602540378443763</v>
       </c>
       <c r="D20" s="61">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9.5854811567261606</v>
       </c>
       <c r="E20" s="61">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-1.403057715734235E-4</v>
       </c>
       <c r="F20" s="60">
         <v>5</v>
       </c>
       <c r="G20" s="63">
-        <f>IF($S$3*$S$4=-1,1,0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I20" s="2"/>
@@ -17787,26 +17795,26 @@
         <v>26</v>
       </c>
       <c r="B21" s="61">
-        <f>((ROUND($L21/10,0))-1)*4+MOD($L21,10)+((J21-1)*16)</f>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="C21" s="61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15.602540378443791</v>
       </c>
       <c r="D21" s="61">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>18.823085463760187</v>
       </c>
       <c r="E21" s="61">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>59.999719388456853</v>
       </c>
       <c r="F21" s="60">
         <v>5</v>
       </c>
       <c r="G21" s="63">
-        <f>IF($S$3*$S$4=-1,1,0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I21" s="2"/>
@@ -17839,26 +17847,26 @@
         <v>26</v>
       </c>
       <c r="B22" s="61">
-        <f>((ROUND($L22/10,0))-1)*4+MOD($L22,10)+((J22-1)*16)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C22" s="61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-0.39745962155618031</v>
       </c>
       <c r="D22" s="61">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9.585481156726182</v>
       </c>
       <c r="E22" s="61">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>119.99957908268468</v>
       </c>
       <c r="F22" s="60">
         <v>5</v>
       </c>
       <c r="G22" s="63">
-        <f>IF($S$3*$S$4=-1,1,0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I22" s="2"/>
@@ -17891,26 +17899,26 @@
         <v>26</v>
       </c>
       <c r="B23" s="61">
-        <f>((ROUND($L23/10,0))-1)*4+MOD($L23,10)+((J23-1)*16)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="C23" s="61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15.60254037844382</v>
       </c>
       <c r="D23" s="61">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-18.127331764375853</v>
       </c>
       <c r="E23" s="61">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>119.99957908268468</v>
       </c>
       <c r="F23" s="60">
         <v>5</v>
       </c>
       <c r="G23" s="63">
-        <f>IF($S$3*$S$4=-1,1,0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I23" s="2"/>
@@ -17943,26 +17951,26 @@
         <v>26</v>
       </c>
       <c r="B24" s="61">
-        <f>((ROUND($L24/10,0))-1)*4+MOD($L24,10)+((J24-1)*16)</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="C24" s="61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-0.39745962155618031</v>
       </c>
       <c r="D24" s="61">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-8.8897274573418343</v>
       </c>
       <c r="E24" s="61">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>59.999719388456853</v>
       </c>
       <c r="F24" s="60">
         <v>5</v>
       </c>
       <c r="G24" s="63">
-        <f>IF($S$3*$S$4=-1,1,0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I24" s="2"/>
@@ -21771,7 +21779,7 @@
   <dimension ref="A1:U55"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6:M8"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21875,7 +21883,7 @@
       </c>
       <c r="O3" s="14">
         <f>+RADIANS(O5)</f>
-        <v>3.1415926535897931</v>
+        <v>-2.0943951023931953</v>
       </c>
       <c r="P3" s="15">
         <v>100</v>
@@ -21963,7 +21971,7 @@
         <v>-2.0943951023932001</v>
       </c>
       <c r="O5" s="3">
-        <v>180</v>
+        <v>-120</v>
       </c>
       <c r="P5" s="41">
         <v>132</v>
@@ -21988,15 +21996,15 @@
       </c>
       <c r="C6" s="61">
         <f t="shared" ref="C6:C8" si="2">((+P6*COS($O$3)-Q6*SIN($O$3)+$O$7)*$S$3)</f>
-        <v>96</v>
+        <v>79.602540378443891</v>
       </c>
       <c r="D6" s="61">
         <f t="shared" ref="D6:D8" si="3">((P6*SIN($O$3)+Q6*COS($O$3)+$O$9)*$S$4)</f>
-        <v>9.7623956929660096</v>
+        <v>19.209438086386086</v>
       </c>
       <c r="E6" s="61">
         <f t="shared" ref="E6:E8" si="4">IF(($S$3*$S$4)=1,1,-1)*(($N6/3.1416*180)+$O$5)</f>
-        <v>120.00014030577157</v>
+        <v>-179.99985969422843</v>
       </c>
       <c r="F6" s="60">
         <v>5</v>
@@ -22047,15 +22055,15 @@
       </c>
       <c r="C7" s="61">
         <f t="shared" si="2"/>
-        <v>95.999999999999972</v>
+        <v>95.602540378443862</v>
       </c>
       <c r="D7" s="61">
         <f t="shared" si="3"/>
-        <v>-8.7128129211019854</v>
+        <v>9.9718337793520959</v>
       </c>
       <c r="E7" s="61">
         <f t="shared" si="4"/>
-        <v>180</v>
+        <v>-120</v>
       </c>
       <c r="F7" s="60">
         <v>5</v>
@@ -22083,7 +22091,8 @@
         <v>0</v>
       </c>
       <c r="O7" s="3">
-        <v>244</v>
+        <f>-37+96</f>
+        <v>59</v>
       </c>
       <c r="P7" s="41">
         <v>148</v>
@@ -22105,15 +22114,15 @@
       </c>
       <c r="C8" s="61">
         <f t="shared" si="2"/>
-        <v>79.999999999999972</v>
+        <v>95.602540378443862</v>
       </c>
       <c r="D8" s="61">
         <f t="shared" si="3"/>
-        <v>-17.950417228135962</v>
+        <v>-8.5033748347159417</v>
       </c>
       <c r="E8" s="61">
         <f t="shared" si="4"/>
-        <v>120.00014030577157</v>
+        <v>-179.99985969422843</v>
       </c>
       <c r="F8" s="60">
         <v>5</v>
@@ -22179,7 +22188,7 @@
         <v>0</v>
       </c>
       <c r="O9" s="3">
-        <v>119</v>
+        <v>202</v>
       </c>
       <c r="P9" s="41">
         <v>164</v>
@@ -22815,7 +22824,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="Q34" sqref="Q34"/>
     </sheetView>
   </sheetViews>
@@ -24785,8 +24794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G165"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G164" sqref="A3:G164"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A103" sqref="A103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27711,15 +27720,15 @@
       </c>
       <c r="C99" s="79">
         <f>IF('4535A_2'!C6="", "", '4535A_2'!C6)</f>
-        <v>96</v>
+        <v>79.602540378443891</v>
       </c>
       <c r="D99" s="79">
         <f>IF('4535A_2'!D6="", "", '4535A_2'!D6)</f>
-        <v>9.7623956929660096</v>
+        <v>19.209438086386086</v>
       </c>
       <c r="E99" s="79">
         <f>IF('4535A_2'!E6="", "", '4535A_2'!E6)</f>
-        <v>120.00014030577157</v>
+        <v>-179.99985969422843</v>
       </c>
       <c r="F99" s="79">
         <f>IF('4535A_2'!F6="", "", '4535A_2'!F6)</f>
@@ -27741,15 +27750,15 @@
       </c>
       <c r="C100" s="79">
         <f>IF('4535A_2'!C7="", "", '4535A_2'!C7)</f>
-        <v>95.999999999999972</v>
+        <v>95.602540378443862</v>
       </c>
       <c r="D100" s="79">
         <f>IF('4535A_2'!D7="", "", '4535A_2'!D7)</f>
-        <v>-8.7128129211019854</v>
+        <v>9.9718337793520959</v>
       </c>
       <c r="E100" s="79">
         <f>IF('4535A_2'!E7="", "", '4535A_2'!E7)</f>
-        <v>180</v>
+        <v>-120</v>
       </c>
       <c r="F100" s="79">
         <f>IF('4535A_2'!F7="", "", '4535A_2'!F7)</f>
@@ -27771,15 +27780,15 @@
       </c>
       <c r="C101" s="79">
         <f>IF('4535A_2'!C8="", "", '4535A_2'!C8)</f>
-        <v>79.999999999999972</v>
+        <v>95.602540378443862</v>
       </c>
       <c r="D101" s="79">
         <f>IF('4535A_2'!D8="", "", '4535A_2'!D8)</f>
-        <v>-17.950417228135962</v>
+        <v>-8.5033748347159417</v>
       </c>
       <c r="E101" s="79">
         <f>IF('4535A_2'!E8="", "", '4535A_2'!E8)</f>
-        <v>120.00014030577157</v>
+        <v>-179.99985969422843</v>
       </c>
       <c r="F101" s="79">
         <f>IF('4535A_2'!F8="", "", '4535A_2'!F8)</f>
@@ -27792,32 +27801,32 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="68" t="str">
-        <f>IF('4535A_2'!A6="", "", '4535A_2'!A6)</f>
-        <v>triangle_10pad</v>
-      </c>
-      <c r="B102" s="79">
-        <f>IF('4535A_2'!B6="", "", '4535A_2'!B6)</f>
-        <v>19</v>
-      </c>
-      <c r="C102" s="79">
-        <f>IF('4535A_2'!C6="", "", '4535A_2'!C6)</f>
-        <v>96</v>
-      </c>
-      <c r="D102" s="79">
-        <f>IF('4535A_2'!D6="", "", '4535A_2'!D6)</f>
-        <v>9.7623956929660096</v>
-      </c>
-      <c r="E102" s="79">
-        <f>IF('4535A_2'!E6="", "", '4535A_2'!E6)</f>
-        <v>120.00014030577157</v>
-      </c>
-      <c r="F102" s="79">
-        <f>IF('4535A_2'!F6="", "", '4535A_2'!F6)</f>
-        <v>5</v>
-      </c>
-      <c r="G102" s="79">
-        <f>IF('4535A_2'!G6="", "", '4535A_2'!G6)</f>
-        <v>0</v>
+        <f>IF('4535A_2'!A9="", "", '4535A_2'!A9)</f>
+        <v/>
+      </c>
+      <c r="B102" s="79" t="str">
+        <f>IF('4535A_2'!B9="", "", '4535A_2'!B9)</f>
+        <v/>
+      </c>
+      <c r="C102" s="79" t="str">
+        <f>IF('4535A_2'!C9="", "", '4535A_2'!C9)</f>
+        <v/>
+      </c>
+      <c r="D102" s="79" t="str">
+        <f>IF('4535A_2'!D9="", "", '4535A_2'!D9)</f>
+        <v/>
+      </c>
+      <c r="E102" s="79" t="str">
+        <f>IF('4535A_2'!E9="", "", '4535A_2'!E9)</f>
+        <v/>
+      </c>
+      <c r="F102" s="79" t="str">
+        <f>IF('4535A_2'!F9="", "", '4535A_2'!F9)</f>
+        <v/>
+      </c>
+      <c r="G102" s="79" t="str">
+        <f>IF('4535A_2'!G9="", "", '4535A_2'!G9)</f>
+        <v/>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fixed triangle positions as per #880 (#889)
</commit_message>
<xml_diff>
--- a/app/skinGui/iniGenerators/rightLeg_Lower_ini_generator.xlsx
+++ b/app/skinGui/iniGenerators/rightLeg_Lower_ini_generator.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\robotologia\icub-main\app\skinGui\iniGenerators\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12585" yWindow="-15" windowWidth="12630" windowHeight="12000" activeTab="5"/>
+    <workbookView xWindow="12585" yWindow="-15" windowWidth="12630" windowHeight="12000" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="4535A" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
     <sheet name="4616A" sheetId="8" r:id="rId7"/>
     <sheet name="final ini" sheetId="5" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -131,7 +136,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -851,6 +856,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -16685,7 +16693,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -16720,7 +16728,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -16932,7 +16940,7 @@
   <dimension ref="A1:U55"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17579,26 +17587,26 @@
         <v>26</v>
       </c>
       <c r="B17" s="61">
-        <f>((ROUND($L17/10,0))-1)*4+MOD($L17,10)+((J17-1)*16)</f>
+        <f t="shared" ref="B17:B24" si="2">((ROUND($L17/10,0))-1)*4+MOD($L17,10)+((J17-1)*16)</f>
         <v>3</v>
       </c>
       <c r="C17" s="61">
-        <f t="shared" ref="C17:C24" si="2">((+P17*COS($O$3)-Q17*SIN($O$3)+$O$7)*$S$3)</f>
+        <f t="shared" ref="C17:C24" si="3">((+P17*COS($O$3)-Q17*SIN($O$3)+$O$7)*$S$3)</f>
         <v>63.602540378443734</v>
       </c>
       <c r="D17" s="61">
-        <f t="shared" ref="D17:D24" si="3">((P17*SIN($O$3)+Q17*COS($O$3)+$O$9)*$S$4)</f>
+        <f t="shared" ref="D17:D24" si="4">((P17*SIN($O$3)+Q17*COS($O$3)+$O$9)*$S$4)</f>
         <v>9.5854811567261606</v>
       </c>
       <c r="E17" s="61">
-        <f t="shared" ref="E17:E24" si="4">IF(($S$3*$S$4)=1,1,-1)*(($N17/3.1416*180)+$O$5)</f>
+        <f t="shared" ref="E17:E24" si="5">IF(($S$3*$S$4)=1,1,-1)*(($N17/3.1416*180)+$O$5)</f>
         <v>-1.403057715734235E-4</v>
       </c>
       <c r="F17" s="60">
         <v>5</v>
       </c>
       <c r="G17" s="63">
-        <f>IF($S$3*$S$4=-1,1,0)</f>
+        <f t="shared" ref="G17:G24" si="6">IF($S$3*$S$4=-1,1,0)</f>
         <v>0</v>
       </c>
       <c r="I17" s="1"/>
@@ -17631,26 +17639,26 @@
         <v>26</v>
       </c>
       <c r="B18" s="61">
-        <f>((ROUND($L18/10,0))-1)*4+MOD($L18,10)+((J18-1)*16)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="C18" s="61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>47.602540378443763</v>
       </c>
       <c r="D18" s="61">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>18.823085463760165</v>
       </c>
       <c r="E18" s="61">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>59.999719388456853</v>
       </c>
       <c r="F18" s="60">
         <v>5</v>
       </c>
       <c r="G18" s="63">
-        <f>IF($S$3*$S$4=-1,1,0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I18" s="1"/>
@@ -17683,26 +17691,26 @@
         <v>26</v>
       </c>
       <c r="B19" s="61">
-        <f>((ROUND($L19/10,0))-1)*4+MOD($L19,10)+((J19-1)*16)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="C19" s="61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>31.602540378443791</v>
       </c>
       <c r="D19" s="61">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-8.8897274573418485</v>
       </c>
       <c r="E19" s="61">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>59.999719388456853</v>
       </c>
       <c r="F19" s="60">
         <v>5</v>
       </c>
       <c r="G19" s="63">
-        <f>IF($S$3*$S$4=-1,1,0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I19" s="1"/>
@@ -17735,26 +17743,26 @@
         <v>26</v>
       </c>
       <c r="B20" s="61">
-        <f>((ROUND($L20/10,0))-1)*4+MOD($L20,10)+((J20-1)*16)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="C20" s="61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>31.602540378443763</v>
       </c>
       <c r="D20" s="61">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9.5854811567261606</v>
       </c>
       <c r="E20" s="61">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-1.403057715734235E-4</v>
       </c>
       <c r="F20" s="60">
         <v>5</v>
       </c>
       <c r="G20" s="63">
-        <f>IF($S$3*$S$4=-1,1,0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I20" s="2"/>
@@ -17787,26 +17795,26 @@
         <v>26</v>
       </c>
       <c r="B21" s="61">
-        <f>((ROUND($L21/10,0))-1)*4+MOD($L21,10)+((J21-1)*16)</f>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="C21" s="61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15.602540378443791</v>
       </c>
       <c r="D21" s="61">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>18.823085463760187</v>
       </c>
       <c r="E21" s="61">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>59.999719388456853</v>
       </c>
       <c r="F21" s="60">
         <v>5</v>
       </c>
       <c r="G21" s="63">
-        <f>IF($S$3*$S$4=-1,1,0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I21" s="2"/>
@@ -17839,26 +17847,26 @@
         <v>26</v>
       </c>
       <c r="B22" s="61">
-        <f>((ROUND($L22/10,0))-1)*4+MOD($L22,10)+((J22-1)*16)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C22" s="61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-0.39745962155618031</v>
       </c>
       <c r="D22" s="61">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9.585481156726182</v>
       </c>
       <c r="E22" s="61">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>119.99957908268468</v>
       </c>
       <c r="F22" s="60">
         <v>5</v>
       </c>
       <c r="G22" s="63">
-        <f>IF($S$3*$S$4=-1,1,0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I22" s="2"/>
@@ -17891,26 +17899,26 @@
         <v>26</v>
       </c>
       <c r="B23" s="61">
-        <f>((ROUND($L23/10,0))-1)*4+MOD($L23,10)+((J23-1)*16)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="C23" s="61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>15.60254037844382</v>
       </c>
       <c r="D23" s="61">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-18.127331764375853</v>
       </c>
       <c r="E23" s="61">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>119.99957908268468</v>
       </c>
       <c r="F23" s="60">
         <v>5</v>
       </c>
       <c r="G23" s="63">
-        <f>IF($S$3*$S$4=-1,1,0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I23" s="2"/>
@@ -17943,26 +17951,26 @@
         <v>26</v>
       </c>
       <c r="B24" s="61">
-        <f>((ROUND($L24/10,0))-1)*4+MOD($L24,10)+((J24-1)*16)</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="C24" s="61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-0.39745962155618031</v>
       </c>
       <c r="D24" s="61">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-8.8897274573418343</v>
       </c>
       <c r="E24" s="61">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>59.999719388456853</v>
       </c>
       <c r="F24" s="60">
         <v>5</v>
       </c>
       <c r="G24" s="63">
-        <f>IF($S$3*$S$4=-1,1,0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I24" s="2"/>
@@ -21771,7 +21779,7 @@
   <dimension ref="A1:U55"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6:M8"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21875,7 +21883,7 @@
       </c>
       <c r="O3" s="14">
         <f>+RADIANS(O5)</f>
-        <v>3.1415926535897931</v>
+        <v>-2.0943951023931953</v>
       </c>
       <c r="P3" s="15">
         <v>100</v>
@@ -21963,7 +21971,7 @@
         <v>-2.0943951023932001</v>
       </c>
       <c r="O5" s="3">
-        <v>180</v>
+        <v>-120</v>
       </c>
       <c r="P5" s="41">
         <v>132</v>
@@ -21988,15 +21996,15 @@
       </c>
       <c r="C6" s="61">
         <f t="shared" ref="C6:C8" si="2">((+P6*COS($O$3)-Q6*SIN($O$3)+$O$7)*$S$3)</f>
-        <v>96</v>
+        <v>79.602540378443891</v>
       </c>
       <c r="D6" s="61">
         <f t="shared" ref="D6:D8" si="3">((P6*SIN($O$3)+Q6*COS($O$3)+$O$9)*$S$4)</f>
-        <v>9.7623956929660096</v>
+        <v>19.209438086386086</v>
       </c>
       <c r="E6" s="61">
         <f t="shared" ref="E6:E8" si="4">IF(($S$3*$S$4)=1,1,-1)*(($N6/3.1416*180)+$O$5)</f>
-        <v>120.00014030577157</v>
+        <v>-179.99985969422843</v>
       </c>
       <c r="F6" s="60">
         <v>5</v>
@@ -22047,15 +22055,15 @@
       </c>
       <c r="C7" s="61">
         <f t="shared" si="2"/>
-        <v>95.999999999999972</v>
+        <v>95.602540378443862</v>
       </c>
       <c r="D7" s="61">
         <f t="shared" si="3"/>
-        <v>-8.7128129211019854</v>
+        <v>9.9718337793520959</v>
       </c>
       <c r="E7" s="61">
         <f t="shared" si="4"/>
-        <v>180</v>
+        <v>-120</v>
       </c>
       <c r="F7" s="60">
         <v>5</v>
@@ -22083,7 +22091,8 @@
         <v>0</v>
       </c>
       <c r="O7" s="3">
-        <v>244</v>
+        <f>-37+96</f>
+        <v>59</v>
       </c>
       <c r="P7" s="41">
         <v>148</v>
@@ -22105,15 +22114,15 @@
       </c>
       <c r="C8" s="61">
         <f t="shared" si="2"/>
-        <v>79.999999999999972</v>
+        <v>95.602540378443862</v>
       </c>
       <c r="D8" s="61">
         <f t="shared" si="3"/>
-        <v>-17.950417228135962</v>
+        <v>-8.5033748347159417</v>
       </c>
       <c r="E8" s="61">
         <f t="shared" si="4"/>
-        <v>120.00014030577157</v>
+        <v>-179.99985969422843</v>
       </c>
       <c r="F8" s="60">
         <v>5</v>
@@ -22179,7 +22188,7 @@
         <v>0</v>
       </c>
       <c r="O9" s="3">
-        <v>119</v>
+        <v>202</v>
       </c>
       <c r="P9" s="41">
         <v>164</v>
@@ -22815,7 +22824,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="Q34" sqref="Q34"/>
     </sheetView>
   </sheetViews>
@@ -24785,8 +24794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G165"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G164" sqref="A3:G164"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A103" sqref="A103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27711,15 +27720,15 @@
       </c>
       <c r="C99" s="79">
         <f>IF('4535A_2'!C6="", "", '4535A_2'!C6)</f>
-        <v>96</v>
+        <v>79.602540378443891</v>
       </c>
       <c r="D99" s="79">
         <f>IF('4535A_2'!D6="", "", '4535A_2'!D6)</f>
-        <v>9.7623956929660096</v>
+        <v>19.209438086386086</v>
       </c>
       <c r="E99" s="79">
         <f>IF('4535A_2'!E6="", "", '4535A_2'!E6)</f>
-        <v>120.00014030577157</v>
+        <v>-179.99985969422843</v>
       </c>
       <c r="F99" s="79">
         <f>IF('4535A_2'!F6="", "", '4535A_2'!F6)</f>
@@ -27741,15 +27750,15 @@
       </c>
       <c r="C100" s="79">
         <f>IF('4535A_2'!C7="", "", '4535A_2'!C7)</f>
-        <v>95.999999999999972</v>
+        <v>95.602540378443862</v>
       </c>
       <c r="D100" s="79">
         <f>IF('4535A_2'!D7="", "", '4535A_2'!D7)</f>
-        <v>-8.7128129211019854</v>
+        <v>9.9718337793520959</v>
       </c>
       <c r="E100" s="79">
         <f>IF('4535A_2'!E7="", "", '4535A_2'!E7)</f>
-        <v>180</v>
+        <v>-120</v>
       </c>
       <c r="F100" s="79">
         <f>IF('4535A_2'!F7="", "", '4535A_2'!F7)</f>
@@ -27771,15 +27780,15 @@
       </c>
       <c r="C101" s="79">
         <f>IF('4535A_2'!C8="", "", '4535A_2'!C8)</f>
-        <v>79.999999999999972</v>
+        <v>95.602540378443862</v>
       </c>
       <c r="D101" s="79">
         <f>IF('4535A_2'!D8="", "", '4535A_2'!D8)</f>
-        <v>-17.950417228135962</v>
+        <v>-8.5033748347159417</v>
       </c>
       <c r="E101" s="79">
         <f>IF('4535A_2'!E8="", "", '4535A_2'!E8)</f>
-        <v>120.00014030577157</v>
+        <v>-179.99985969422843</v>
       </c>
       <c r="F101" s="79">
         <f>IF('4535A_2'!F8="", "", '4535A_2'!F8)</f>
@@ -27792,32 +27801,32 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="68" t="str">
-        <f>IF('4535A_2'!A6="", "", '4535A_2'!A6)</f>
-        <v>triangle_10pad</v>
-      </c>
-      <c r="B102" s="79">
-        <f>IF('4535A_2'!B6="", "", '4535A_2'!B6)</f>
-        <v>19</v>
-      </c>
-      <c r="C102" s="79">
-        <f>IF('4535A_2'!C6="", "", '4535A_2'!C6)</f>
-        <v>96</v>
-      </c>
-      <c r="D102" s="79">
-        <f>IF('4535A_2'!D6="", "", '4535A_2'!D6)</f>
-        <v>9.7623956929660096</v>
-      </c>
-      <c r="E102" s="79">
-        <f>IF('4535A_2'!E6="", "", '4535A_2'!E6)</f>
-        <v>120.00014030577157</v>
-      </c>
-      <c r="F102" s="79">
-        <f>IF('4535A_2'!F6="", "", '4535A_2'!F6)</f>
-        <v>5</v>
-      </c>
-      <c r="G102" s="79">
-        <f>IF('4535A_2'!G6="", "", '4535A_2'!G6)</f>
-        <v>0</v>
+        <f>IF('4535A_2'!A9="", "", '4535A_2'!A9)</f>
+        <v/>
+      </c>
+      <c r="B102" s="79" t="str">
+        <f>IF('4535A_2'!B9="", "", '4535A_2'!B9)</f>
+        <v/>
+      </c>
+      <c r="C102" s="79" t="str">
+        <f>IF('4535A_2'!C9="", "", '4535A_2'!C9)</f>
+        <v/>
+      </c>
+      <c r="D102" s="79" t="str">
+        <f>IF('4535A_2'!D9="", "", '4535A_2'!D9)</f>
+        <v/>
+      </c>
+      <c r="E102" s="79" t="str">
+        <f>IF('4535A_2'!E9="", "", '4535A_2'!E9)</f>
+        <v/>
+      </c>
+      <c r="F102" s="79" t="str">
+        <f>IF('4535A_2'!F9="", "", '4535A_2'!F9)</f>
+        <v/>
+      </c>
+      <c r="G102" s="79" t="str">
+        <f>IF('4535A_2'!G9="", "", '4535A_2'!G9)</f>
+        <v/>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>